<commit_message>
mise à jour du word_service.py
</commit_message>
<xml_diff>
--- a/backend/uploads/modified_file.xlsx
+++ b/backend/uploads/modified_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndyVESPUCE\bulletin-espi\backend\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DAC356-4341-416B-A151-5368386C425B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA9181B-8822-4013-8BB4-E26D9CFEA5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="385">
   <si>
     <t>L-M1 MAPI ALT 1 - ALT Semestre 1</t>
   </si>
@@ -763,240 +763,240 @@
     <t>26/11/2002</t>
   </si>
   <si>
+    <t>LE GALL Zoé</t>
+  </si>
+  <si>
+    <t>17 (0,3) - 12,5 (0,7)</t>
+  </si>
+  <si>
+    <t>15,5 (0,4) - 15 (0,6)</t>
+  </si>
+  <si>
+    <t>16 (0,25) - 16 (0,25) - 15 (0,25) - 16,5 (0,25)</t>
+  </si>
+  <si>
+    <t>16,75</t>
+  </si>
+  <si>
+    <t>13,5 - 15</t>
+  </si>
+  <si>
+    <t>16 (0,5) - 17,5</t>
+  </si>
+  <si>
+    <t>15,06 (18)</t>
+  </si>
+  <si>
+    <t>27/09/2002</t>
+  </si>
+  <si>
+    <t>LEMAHIEU Carole</t>
+  </si>
+  <si>
+    <t>18 (0,3) - 13,5</t>
+  </si>
+  <si>
+    <t>13,5 (0,4) - 15 (0,6)</t>
+  </si>
+  <si>
+    <t>16 (0,25) - 15,5 (0,25) - 11 (0,25) - 20 (0,25)</t>
+  </si>
+  <si>
+    <t>00h30</t>
+  </si>
+  <si>
+    <t>16 (5)</t>
+  </si>
+  <si>
+    <t>15/06/2001</t>
+  </si>
+  <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>MAAROUF Adda</t>
+  </si>
+  <si>
+    <t>14 (0,3) - 11,5</t>
+  </si>
+  <si>
+    <t>15,75 (0,3) - 13,75 (0,7)</t>
+  </si>
+  <si>
+    <t>15,5</t>
+  </si>
+  <si>
+    <t>15,25 (0,4) - 14 (0,6)</t>
+  </si>
+  <si>
+    <t>14 (0,25) - 15,5 (0,25) - 15 (0,25) - 20 (0,25)</t>
+  </si>
+  <si>
+    <t>13 (0,5) - 15</t>
+  </si>
+  <si>
+    <t>14,66 (25)</t>
+  </si>
+  <si>
+    <t>30/12/2001</t>
+  </si>
+  <si>
+    <t>6h00</t>
+  </si>
+  <si>
+    <t>1h00</t>
+  </si>
+  <si>
+    <t>MATIAS Léonie</t>
+  </si>
+  <si>
+    <t>13,5 (0,3) - 18,5</t>
+  </si>
+  <si>
+    <t>17 (0,3) - 13,75 (0,7)</t>
+  </si>
+  <si>
+    <t>14,5 (0,4) - 14 (0,6)</t>
+  </si>
+  <si>
+    <t>14 (0,25) - 15,5 (0,25) - 16 (0,25) - 2 (0,25)</t>
+  </si>
+  <si>
+    <t>15,21 (17)</t>
+  </si>
+  <si>
+    <t>19/07/2002</t>
+  </si>
+  <si>
+    <t>MORAND Dylan</t>
+  </si>
+  <si>
+    <t>11 (10,3) - 8</t>
+  </si>
+  <si>
+    <t>16,25 (0,3) - 13,5 (0,7)</t>
+  </si>
+  <si>
+    <t>10 (0,4) - 11,5 (0,6)</t>
+  </si>
+  <si>
+    <t>15,5 (0,6) - 11 (0,4)</t>
+  </si>
+  <si>
+    <t>14 (0,25) - 12 (0,25) - 11 (0,25) - 20 (0,25)</t>
+  </si>
+  <si>
+    <t>10,66</t>
+  </si>
+  <si>
+    <t>10,25</t>
+  </si>
+  <si>
+    <t>16 (0,5) - 15</t>
+  </si>
+  <si>
+    <t>14,28 (33)</t>
+  </si>
+  <si>
+    <t>12/11/2001</t>
+  </si>
+  <si>
+    <t>NOLOT Juliette</t>
+  </si>
+  <si>
+    <t>14 (0,3) - 17,5</t>
+  </si>
+  <si>
+    <t>16,25 (0,3) - 14 (0,7)</t>
+  </si>
+  <si>
+    <t>14,5 (0,6) - 14 (0,4)</t>
+  </si>
+  <si>
+    <t>15 (0,25) - 14,5 (0,25) - 9 (0,25) - 20 (0,25)</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>16 (0,5) - 16,5</t>
+  </si>
+  <si>
+    <t>15,41 (13)</t>
+  </si>
+  <si>
+    <t>24/11/2000</t>
+  </si>
+  <si>
+    <t>PINGET Nicolas</t>
+  </si>
+  <si>
+    <t>13 (0,3) - 17</t>
+  </si>
+  <si>
+    <t>16 (0,3) - 16,75 (0,7)</t>
+  </si>
+  <si>
+    <t>15 (0,25) - 16,5 (0,25) - 9 (0,25) - 20 (0,25)</t>
+  </si>
+  <si>
+    <t>19,5</t>
+  </si>
+  <si>
+    <t>15 (0,5) - 17</t>
+  </si>
+  <si>
+    <t>16,22 (3)</t>
+  </si>
+  <si>
+    <t>04/09/1996</t>
+  </si>
+  <si>
+    <t>REYMOND Enzo</t>
+  </si>
+  <si>
+    <t>12,5 (10,3) - 10,5</t>
+  </si>
+  <si>
+    <t>15,75 (0,3) - 12,5 (0,7)</t>
+  </si>
+  <si>
+    <t>11 (0,4) - 13 (0,6)</t>
+  </si>
+  <si>
+    <t>12 (0,6) - 10 (0,4)</t>
+  </si>
+  <si>
+    <t>14,5 (0,25) - 12 (0,25) - 14 (0,25) - 20 (0,25)</t>
+  </si>
+  <si>
+    <t>12,66</t>
+  </si>
+  <si>
+    <t>15 (0,5) - 13</t>
+  </si>
+  <si>
+    <t>13,75 (43)</t>
+  </si>
+  <si>
+    <t>04/09/2002</t>
+  </si>
+  <si>
+    <t>4h15</t>
+  </si>
+  <si>
+    <t>23 minutes</t>
+  </si>
+  <si>
+    <t>SIMONDET Floriane</t>
+  </si>
+  <si>
+    <t>0 (3) - 0</t>
+  </si>
+  <si>
     <t>18h00</t>
   </si>
   <si>
-    <t>LE GALL Zoé</t>
-  </si>
-  <si>
-    <t>17 (0,3) - 12,5 (0,7)</t>
-  </si>
-  <si>
-    <t>15,5 (0,4) - 15 (0,6)</t>
-  </si>
-  <si>
-    <t>16 (0,25) - 16 (0,25) - 15 (0,25) - 16,5 (0,25)</t>
-  </si>
-  <si>
-    <t>16,75</t>
-  </si>
-  <si>
-    <t>13,5 - 15</t>
-  </si>
-  <si>
-    <t>16 (0,5) - 17,5</t>
-  </si>
-  <si>
-    <t>15,06 (18)</t>
-  </si>
-  <si>
-    <t>27/09/2002</t>
-  </si>
-  <si>
-    <t>LEMAHIEU Carole</t>
-  </si>
-  <si>
-    <t>18 (0,3) - 13,5</t>
-  </si>
-  <si>
-    <t>13,5 (0,4) - 15 (0,6)</t>
-  </si>
-  <si>
-    <t>16 (0,25) - 15,5 (0,25) - 11 (0,25) - 20 (0,25)</t>
-  </si>
-  <si>
-    <t>00h30</t>
-  </si>
-  <si>
-    <t>16 (5)</t>
-  </si>
-  <si>
-    <t>15/06/2001</t>
-  </si>
-  <si>
-    <t>2h30</t>
-  </si>
-  <si>
-    <t>MAAROUF Adda</t>
-  </si>
-  <si>
-    <t>14 (0,3) - 11,5</t>
-  </si>
-  <si>
-    <t>15,75 (0,3) - 13,75 (0,7)</t>
-  </si>
-  <si>
-    <t>15,5</t>
-  </si>
-  <si>
-    <t>15,25 (0,4) - 14 (0,6)</t>
-  </si>
-  <si>
-    <t>14 (0,25) - 15,5 (0,25) - 15 (0,25) - 20 (0,25)</t>
-  </si>
-  <si>
-    <t>13 (0,5) - 15</t>
-  </si>
-  <si>
-    <t>14,66 (25)</t>
-  </si>
-  <si>
-    <t>30/12/2001</t>
-  </si>
-  <si>
-    <t>6h00</t>
-  </si>
-  <si>
-    <t>1h00</t>
-  </si>
-  <si>
-    <t>MATIAS Léonie</t>
-  </si>
-  <si>
-    <t>13,5 (0,3) - 18,5</t>
-  </si>
-  <si>
-    <t>17 (0,3) - 13,75 (0,7)</t>
-  </si>
-  <si>
-    <t>14,5 (0,4) - 14 (0,6)</t>
-  </si>
-  <si>
-    <t>14 (0,25) - 15,5 (0,25) - 16 (0,25) - 2 (0,25)</t>
-  </si>
-  <si>
-    <t>15,21 (17)</t>
-  </si>
-  <si>
-    <t>19/07/2002</t>
-  </si>
-  <si>
-    <t>MORAND Dylan</t>
-  </si>
-  <si>
-    <t>11 (10,3) - 8</t>
-  </si>
-  <si>
-    <t>16,25 (0,3) - 13,5 (0,7)</t>
-  </si>
-  <si>
-    <t>10 (0,4) - 11,5 (0,6)</t>
-  </si>
-  <si>
-    <t>15,5 (0,6) - 11 (0,4)</t>
-  </si>
-  <si>
-    <t>14 (0,25) - 12 (0,25) - 11 (0,25) - 20 (0,25)</t>
-  </si>
-  <si>
-    <t>10,66</t>
-  </si>
-  <si>
-    <t>10,25</t>
-  </si>
-  <si>
-    <t>16 (0,5) - 15</t>
-  </si>
-  <si>
-    <t>14,28 (33)</t>
-  </si>
-  <si>
-    <t>12/11/2001</t>
-  </si>
-  <si>
-    <t>NOLOT Juliette</t>
-  </si>
-  <si>
-    <t>14 (0,3) - 17,5</t>
-  </si>
-  <si>
-    <t>16,25 (0,3) - 14 (0,7)</t>
-  </si>
-  <si>
-    <t>14,5 (0,6) - 14 (0,4)</t>
-  </si>
-  <si>
-    <t>15 (0,25) - 14,5 (0,25) - 9 (0,25) - 20 (0,25)</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>16 (0,5) - 16,5</t>
-  </si>
-  <si>
-    <t>15,41 (13)</t>
-  </si>
-  <si>
-    <t>24/11/2000</t>
-  </si>
-  <si>
-    <t>PINGET Nicolas</t>
-  </si>
-  <si>
-    <t>13 (0,3) - 17</t>
-  </si>
-  <si>
-    <t>16 (0,3) - 16,75 (0,7)</t>
-  </si>
-  <si>
-    <t>15 (0,25) - 16,5 (0,25) - 9 (0,25) - 20 (0,25)</t>
-  </si>
-  <si>
-    <t>19,5</t>
-  </si>
-  <si>
-    <t>15 (0,5) - 17</t>
-  </si>
-  <si>
-    <t>16,22 (3)</t>
-  </si>
-  <si>
-    <t>04/09/1996</t>
-  </si>
-  <si>
-    <t>REYMOND Enzo</t>
-  </si>
-  <si>
-    <t>12,5 (10,3) - 10,5</t>
-  </si>
-  <si>
-    <t>15,75 (0,3) - 12,5 (0,7)</t>
-  </si>
-  <si>
-    <t>11 (0,4) - 13 (0,6)</t>
-  </si>
-  <si>
-    <t>12 (0,6) - 10 (0,4)</t>
-  </si>
-  <si>
-    <t>14,5 (0,25) - 12 (0,25) - 14 (0,25) - 20 (0,25)</t>
-  </si>
-  <si>
-    <t>12,66</t>
-  </si>
-  <si>
-    <t>15 (0,5) - 13</t>
-  </si>
-  <si>
-    <t>13,75 (43)</t>
-  </si>
-  <si>
-    <t>04/09/2002</t>
-  </si>
-  <si>
-    <t>4h15</t>
-  </si>
-  <si>
-    <t>23 minutes</t>
-  </si>
-  <si>
-    <t>SIMONDET Floriane</t>
-  </si>
-  <si>
-    <t>0 (3) - 0</t>
-  </si>
-  <si>
     <t>Absent au devoir (0,3)</t>
   </si>
   <si>
@@ -1030,7 +1030,7 @@
     <t>18/04/1996</t>
   </si>
   <si>
-    <t>212h30</t>
+    <t>224h30</t>
   </si>
   <si>
     <t>SZOSTAK Tom</t>
@@ -1115,9 +1115,6 @@
   </si>
   <si>
     <t>22h00</t>
-  </si>
-  <si>
-    <t>3h00</t>
   </si>
   <si>
     <t>4 minutes</t>
@@ -1905,13 +1902,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BU34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BF1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="BQ5" sqref="BQ5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="0.88671875" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
@@ -1974,7 +1971,6 @@
     <col min="61" max="61" width="5" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="6" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="9" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:73" ht="4.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4916,7 +4912,7 @@
         <v>51</v>
       </c>
       <c r="BT21" t="s">
-        <v>247</v>
+        <v>142</v>
       </c>
       <c r="BU21" t="s">
         <v>51</v>
@@ -4927,7 +4923,7 @@
         <v>72859</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="2">
@@ -4949,7 +4945,7 @@
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M22" s="2">
         <v>2</v>
@@ -4975,7 +4971,7 @@
       </c>
       <c r="W22" s="2"/>
       <c r="X22" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Y22" s="2">
         <v>2</v>
@@ -4994,7 +4990,7 @@
       </c>
       <c r="AF22" s="2"/>
       <c r="AG22" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AH22" s="2">
         <v>2</v>
@@ -5017,7 +5013,7 @@
       <c r="AT22" s="2"/>
       <c r="AU22" s="2"/>
       <c r="AV22" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AW22" s="2"/>
       <c r="AX22" s="2"/>
@@ -5027,7 +5023,7 @@
       </c>
       <c r="BA22" s="2"/>
       <c r="BB22" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BC22" s="2">
         <v>2</v>
@@ -5041,14 +5037,14 @@
       </c>
       <c r="BG22" s="2"/>
       <c r="BH22" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="BI22" s="2">
         <v>2</v>
       </c>
       <c r="BJ22" s="24"/>
       <c r="BK22" s="29" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BL22" s="2">
         <v>19</v>
@@ -5057,7 +5053,7 @@
         <v>104</v>
       </c>
       <c r="BN22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BO22" t="s">
         <v>53</v>
@@ -5086,7 +5082,7 @@
         <v>89301</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="4">
@@ -5101,7 +5097,7 @@
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J23" s="4">
         <v>2</v>
@@ -5132,7 +5128,7 @@
       </c>
       <c r="W23" s="4"/>
       <c r="X23" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Y23" s="4">
         <v>2</v>
@@ -5151,7 +5147,7 @@
       </c>
       <c r="AF23" s="4"/>
       <c r="AG23" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AH23" s="4">
         <v>2</v>
@@ -5194,7 +5190,7 @@
         <v>2</v>
       </c>
       <c r="BD23" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BE23" s="5" t="s">
         <v>92</v>
@@ -5211,16 +5207,16 @@
       </c>
       <c r="BJ23" s="23"/>
       <c r="BK23" s="28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="BL23" s="4">
         <v>28</v>
       </c>
       <c r="BM23" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BN23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="BO23" t="s">
         <v>53</v>
@@ -5235,10 +5231,10 @@
         <v>55</v>
       </c>
       <c r="BS23" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="BT23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="BU23" t="s">
         <v>51</v>
@@ -5249,7 +5245,7 @@
         <v>85405</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="2">
@@ -5264,14 +5260,14 @@
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J24" s="2">
         <v>2</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M24" s="2">
         <v>2</v>
@@ -5283,7 +5279,7 @@
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="S24" s="2">
         <v>3</v>
@@ -5297,7 +5293,7 @@
       </c>
       <c r="W24" s="2"/>
       <c r="X24" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Y24" s="2">
         <v>2</v>
@@ -5318,7 +5314,7 @@
       </c>
       <c r="AF24" s="2"/>
       <c r="AG24" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AH24" s="2">
         <v>2</v>
@@ -5353,7 +5349,7 @@
       </c>
       <c r="BA24" s="2"/>
       <c r="BB24" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BC24" s="2">
         <v>2</v>
@@ -5367,14 +5363,14 @@
       </c>
       <c r="BG24" s="2"/>
       <c r="BH24" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="BI24" s="2">
         <v>2</v>
       </c>
       <c r="BJ24" s="24"/>
       <c r="BK24" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="BL24" s="2">
         <v>28</v>
@@ -5383,7 +5379,7 @@
         <v>135</v>
       </c>
       <c r="BN24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="BO24" t="s">
         <v>53</v>
@@ -5398,10 +5394,10 @@
         <v>55</v>
       </c>
       <c r="BS24" t="s">
+        <v>273</v>
+      </c>
+      <c r="BT24" t="s">
         <v>274</v>
-      </c>
-      <c r="BT24" t="s">
-        <v>275</v>
       </c>
       <c r="BU24" t="s">
         <v>51</v>
@@ -5412,7 +5408,7 @@
         <v>85382</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="4">
@@ -5427,14 +5423,14 @@
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J25" s="4">
         <v>2</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M25" s="4">
         <v>2</v>
@@ -5458,7 +5454,7 @@
       </c>
       <c r="W25" s="4"/>
       <c r="X25" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y25" s="4">
         <v>2</v>
@@ -5477,7 +5473,7 @@
       </c>
       <c r="AF25" s="4"/>
       <c r="AG25" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AH25" s="4">
         <v>2</v>
@@ -5512,7 +5508,7 @@
       </c>
       <c r="BA25" s="4"/>
       <c r="BB25" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BC25" s="4">
         <v>2</v>
@@ -5533,7 +5529,7 @@
       </c>
       <c r="BJ25" s="23"/>
       <c r="BK25" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="BL25" s="4">
         <v>28</v>
@@ -5542,7 +5538,7 @@
         <v>104</v>
       </c>
       <c r="BN25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="BO25" t="s">
         <v>53</v>
@@ -5571,7 +5567,7 @@
         <v>85406</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="2">
@@ -5586,14 +5582,14 @@
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J26" s="2">
         <v>2</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M26" s="2">
         <v>2</v>
@@ -5617,14 +5613,14 @@
       </c>
       <c r="W26" s="2"/>
       <c r="X26" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Y26" s="2">
         <v>2</v>
       </c>
       <c r="Z26" s="2"/>
       <c r="AA26" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AB26" s="2">
         <v>2</v>
@@ -5636,7 +5632,7 @@
       </c>
       <c r="AF26" s="2"/>
       <c r="AG26" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AH26" s="2">
         <v>2</v>
@@ -5651,7 +5647,7 @@
       <c r="AN26" s="2"/>
       <c r="AO26" s="2"/>
       <c r="AP26" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AQ26" s="2"/>
       <c r="AR26" s="2"/>
@@ -5663,7 +5659,7 @@
       </c>
       <c r="AU26" s="2"/>
       <c r="AV26" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AW26" s="2"/>
       <c r="AX26" s="2"/>
@@ -5687,14 +5683,14 @@
       </c>
       <c r="BG26" s="2"/>
       <c r="BH26" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="BI26" s="2">
         <v>2</v>
       </c>
       <c r="BJ26" s="24"/>
       <c r="BK26" s="29" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="BL26" s="2">
         <v>28</v>
@@ -5703,7 +5699,7 @@
         <v>68</v>
       </c>
       <c r="BN26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="BO26" t="s">
         <v>53</v>
@@ -5732,7 +5728,7 @@
         <v>85784</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="4">
@@ -5747,14 +5743,14 @@
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J27" s="4">
         <v>2</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M27" s="4">
         <v>2</v>
@@ -5778,14 +5774,14 @@
       </c>
       <c r="W27" s="4"/>
       <c r="X27" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Y27" s="4">
         <v>2</v>
       </c>
       <c r="Z27" s="4"/>
       <c r="AA27" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AB27" s="4">
         <v>2</v>
@@ -5797,7 +5793,7 @@
       </c>
       <c r="AF27" s="4"/>
       <c r="AG27" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AH27" s="4">
         <v>2</v>
@@ -5812,7 +5808,7 @@
       <c r="AN27" s="4"/>
       <c r="AO27" s="4"/>
       <c r="AP27" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AQ27" s="4"/>
       <c r="AR27" s="4"/>
@@ -5848,14 +5844,14 @@
       </c>
       <c r="BG27" s="4"/>
       <c r="BH27" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="BI27" s="4">
         <v>2</v>
       </c>
       <c r="BJ27" s="23"/>
       <c r="BK27" s="28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="BL27" s="4">
         <v>28</v>
@@ -5864,7 +5860,7 @@
         <v>51</v>
       </c>
       <c r="BN27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="BO27" t="s">
         <v>53</v>
@@ -5882,7 +5878,7 @@
         <v>51</v>
       </c>
       <c r="BT27" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="BU27" t="s">
         <v>51</v>
@@ -5893,7 +5889,7 @@
         <v>85357</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="2">
@@ -5908,14 +5904,14 @@
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J28" s="2">
         <v>2</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M28" s="2">
         <v>2</v>
@@ -5939,7 +5935,7 @@
       </c>
       <c r="W28" s="2"/>
       <c r="X28" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y28" s="2">
         <v>2</v>
@@ -5958,7 +5954,7 @@
       </c>
       <c r="AF28" s="2"/>
       <c r="AG28" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AH28" s="2">
         <v>2</v>
@@ -5978,7 +5974,7 @@
       <c r="AQ28" s="2"/>
       <c r="AR28" s="2"/>
       <c r="AS28" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AT28" s="2">
         <v>9</v>
@@ -6009,14 +6005,14 @@
       </c>
       <c r="BG28" s="2"/>
       <c r="BH28" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="BI28" s="2">
         <v>2</v>
       </c>
       <c r="BJ28" s="24"/>
       <c r="BK28" s="29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="BL28" s="2">
         <v>28</v>
@@ -6025,7 +6021,7 @@
         <v>51</v>
       </c>
       <c r="BN28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="BO28" t="s">
         <v>53</v>
@@ -6043,7 +6039,7 @@
         <v>51</v>
       </c>
       <c r="BT28" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
       <c r="BU28" t="s">
         <v>51</v>
@@ -6054,7 +6050,7 @@
         <v>85712</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="4">
@@ -6069,14 +6065,14 @@
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J29" s="4">
         <v>2</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M29" s="4">
         <v>2</v>
@@ -6100,14 +6096,14 @@
       </c>
       <c r="W29" s="4"/>
       <c r="X29" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Y29" s="4">
         <v>2</v>
       </c>
       <c r="Z29" s="4"/>
       <c r="AA29" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AB29" s="4">
         <v>2</v>
@@ -6119,7 +6115,7 @@
       </c>
       <c r="AF29" s="4"/>
       <c r="AG29" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AH29" s="4">
         <v>2</v>
@@ -6134,7 +6130,7 @@
       <c r="AN29" s="4"/>
       <c r="AO29" s="4"/>
       <c r="AP29" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AQ29" s="4"/>
       <c r="AR29" s="4"/>
@@ -6172,14 +6168,14 @@
       </c>
       <c r="BG29" s="4"/>
       <c r="BH29" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="BI29" s="4">
         <v>2</v>
       </c>
       <c r="BJ29" s="23"/>
       <c r="BK29" s="28" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="BL29" s="4">
         <v>25</v>
@@ -6188,7 +6184,7 @@
         <v>237</v>
       </c>
       <c r="BN29" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="BO29" t="s">
         <v>53</v>
@@ -6206,10 +6202,10 @@
         <v>51</v>
       </c>
       <c r="BT29" t="s">
+        <v>320</v>
+      </c>
+      <c r="BU29" t="s">
         <v>321</v>
-      </c>
-      <c r="BU29" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:73" x14ac:dyDescent="0.3">
@@ -6217,7 +6213,7 @@
         <v>157671</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="2">
@@ -6225,20 +6221,20 @@
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G30" s="2">
         <v>0</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>247</v>
+        <v>324</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>325</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
-        <v>247</v>
+        <v>324</v>
       </c>
       <c r="L30" s="3" t="s">
         <v>326</v>
@@ -6327,7 +6323,7 @@
       </c>
       <c r="BI30" s="2"/>
       <c r="BJ30" s="24" t="s">
-        <v>247</v>
+        <v>324</v>
       </c>
       <c r="BK30" s="29" t="s">
         <v>333</v>
@@ -6602,7 +6598,7 @@
       </c>
       <c r="AF32" s="2"/>
       <c r="AG32" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AH32" s="2">
         <v>2</v>
@@ -6629,7 +6625,7 @@
       </c>
       <c r="AU32" s="2"/>
       <c r="AV32" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AW32" s="2"/>
       <c r="AX32" s="2"/>
@@ -6858,53 +6854,53 @@
         <v>364</v>
       </c>
       <c r="BT33" t="s">
+        <v>126</v>
+      </c>
+      <c r="BU33" t="s">
         <v>365</v>
-      </c>
-      <c r="BU33" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="34" spans="1:73" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>367</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>368</v>
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
       <c r="F34" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G34" s="17"/>
       <c r="H34" s="17"/>
       <c r="I34" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J34" s="17"/>
       <c r="K34" s="17"/>
       <c r="L34" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
       <c r="O34" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="P34" s="17"/>
       <c r="Q34" s="17"/>
       <c r="R34" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="S34" s="17"/>
       <c r="T34" s="17"/>
       <c r="U34" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="V34" s="17"/>
       <c r="W34" s="17"/>
       <c r="X34" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Y34" s="17"/>
       <c r="Z34" s="17"/>
@@ -6914,12 +6910,12 @@
       <c r="AB34" s="17"/>
       <c r="AC34" s="17"/>
       <c r="AD34" s="17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AE34" s="17"/>
       <c r="AF34" s="17"/>
       <c r="AG34" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AH34" s="17"/>
       <c r="AI34" s="17"/>
@@ -6927,47 +6923,47 @@
       <c r="AK34" s="17"/>
       <c r="AL34" s="17"/>
       <c r="AM34" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AN34" s="17"/>
       <c r="AO34" s="17"/>
       <c r="AP34" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AQ34" s="17"/>
       <c r="AR34" s="17"/>
       <c r="AS34" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AT34" s="17"/>
       <c r="AU34" s="17"/>
       <c r="AV34" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AW34" s="17"/>
       <c r="AX34" s="17"/>
       <c r="AY34" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AZ34" s="17"/>
       <c r="BA34" s="17"/>
       <c r="BB34" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="BC34" s="17"/>
       <c r="BD34" s="17"/>
       <c r="BE34" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="BF34" s="17"/>
       <c r="BG34" s="17"/>
       <c r="BH34" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="BI34" s="17"/>
       <c r="BJ34" s="25"/>
       <c r="BK34" s="30" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="BL34" s="17"/>
       <c r="BM34" s="20"/>

</xml_diff>